<commit_message>
Modify config.xlsx for IEX
</commit_message>
<xml_diff>
--- a/Shiny-IEX/config.xlsx
+++ b/Shiny-IEX/config.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DCOLANTO\OneDrive - Environmental Protection Agency (EPA)\Profile\Desktop\IEX_2-20-24\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/burkhardt_jonathan_epa_gov/Documents/Profile/Desktop/Git/Water_Treatment_Models/Shiny-IEX/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A774DBF-292C-4191-B0AC-FF53BCE933BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{1A02411E-970A-4A87-9231-9B3561140CA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="1100" windowWidth="14400" windowHeight="7270" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30750" yWindow="4275" windowWidth="38700" windowHeight="15285" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" r:id="rId1"/>
@@ -513,9 +513,9 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -526,7 +526,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -537,7 +537,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -548,7 +548,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -559,7 +559,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -570,7 +570,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -581,7 +581,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -592,7 +592,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -603,7 +603,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -611,7 +611,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -622,7 +622,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -642,16 +642,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G3:G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -686,7 +686,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -721,7 +721,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -741,7 +741,7 @@
         <v>10</v>
       </c>
       <c r="G3" s="1">
-        <v>2E-8</v>
+        <v>1.9999999999999999E-7</v>
       </c>
       <c r="H3" t="s">
         <v>31</v>
@@ -756,7 +756,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -776,7 +776,7 @@
         <v>10</v>
       </c>
       <c r="G4" s="1">
-        <v>2E-8</v>
+        <v>1.9999999999999999E-7</v>
       </c>
       <c r="H4" t="s">
         <v>31</v>
@@ -791,7 +791,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -811,7 +811,7 @@
         <v>10</v>
       </c>
       <c r="G5" s="1">
-        <v>2E-8</v>
+        <v>1.9999999999999999E-7</v>
       </c>
       <c r="H5" t="s">
         <v>31</v>
@@ -826,7 +826,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -874,9 +874,9 @@
       <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -896,7 +896,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -916,7 +916,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>40.5</v>
       </c>
@@ -950,9 +950,9 @@
       <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -960,7 +960,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -977,18 +977,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CC5EA50-FE9E-4A25-997F-AD599316F020}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>36</v>
       </c>

</xml_diff>